<commit_message>
Added 5 Coaches profile file to explore; Simulación Montecarlo con árbitros
</commit_message>
<xml_diff>
--- a/Coaches_carreers/Coaches_xValues/coaches_results.xlsx
+++ b/Coaches_carreers/Coaches_xValues/coaches_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\La Cima del Éxito\Futbol\Coaches_carreers\Coaches_xValues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159A6462-BDFC-43DD-9B9D-A6A109250DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2727C2D-21AE-4C10-832F-3C0A84CA1D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -662,6 +662,36 @@
   </cellStyles>
   <dxfs count="23">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -696,6 +726,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -703,39 +736,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -768,6 +768,20 @@
       </font>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -796,20 +810,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -824,7 +824,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E30418-5C00-4CF3-BA1D-8700EDD2F295}" name="Table1" displayName="Table1" ref="A1:BV26" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E30418-5C00-4CF3-BA1D-8700EDD2F295}" name="Table1" displayName="Table1" ref="A1:BV26" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="A1:BV26" xr:uid="{82E30418-5C00-4CF3-BA1D-8700EDD2F295}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BV26">
     <sortCondition descending="1" ref="BR1:BR26"/>
@@ -844,16 +844,16 @@
     <tableColumn id="2" xr3:uid="{FB68427F-DF95-424C-8E3E-BDD98B699A56}" name="matches"/>
     <tableColumn id="3" xr3:uid="{F1B65ABD-A5E1-467C-97CF-620A719C635B}" name="matchesH"/>
     <tableColumn id="4" xr3:uid="{453AE61C-1ED4-4317-8E7C-D2B9A524696F}" name="matchesA"/>
-    <tableColumn id="5" xr3:uid="{777813C9-454A-4370-A6FC-1459C3C0CD20}" name="rPoints" dataDxfId="16" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{777813C9-454A-4370-A6FC-1459C3C0CD20}" name="rPoints" dataDxfId="19" dataCellStyle="Percent"/>
     <tableColumn id="6" xr3:uid="{D4C5F585-A38D-4AFA-8092-6B2D2538C088}" name="Points"/>
     <tableColumn id="7" xr3:uid="{2EB8B8F8-C0AA-47CD-982B-9FE1EEE73A46}" name="xPoints"/>
-    <tableColumn id="8" xr3:uid="{A7A70B24-98BC-4703-85D9-F6BF5177B11A}" name="rPointsH" dataDxfId="17" dataCellStyle="Percent"/>
+    <tableColumn id="8" xr3:uid="{A7A70B24-98BC-4703-85D9-F6BF5177B11A}" name="rPointsH" dataDxfId="18" dataCellStyle="Percent"/>
     <tableColumn id="9" xr3:uid="{1D5C626B-6EBD-405B-8F2C-8C73D291B811}" name="PointsH"/>
     <tableColumn id="10" xr3:uid="{E41CC8DF-A485-4740-8B78-13CBFE268B9B}" name="xPointsH"/>
-    <tableColumn id="11" xr3:uid="{8B61851F-BCE2-4EE3-982A-E2BE245D2DD4}" name="rPointsA" dataDxfId="18" dataCellStyle="Percent"/>
+    <tableColumn id="11" xr3:uid="{8B61851F-BCE2-4EE3-982A-E2BE245D2DD4}" name="rPointsA" dataDxfId="17" dataCellStyle="Percent"/>
     <tableColumn id="12" xr3:uid="{843F2F78-38C5-4600-AA90-9978BDAA5659}" name="PointsA"/>
     <tableColumn id="13" xr3:uid="{C6A8C0BF-1831-438C-9B78-12B3EFC282A8}" name="xPointsA"/>
-    <tableColumn id="14" xr3:uid="{5C9CD898-18DE-4A41-991C-EA7AFA3E2AE6}" name="rWins" dataDxfId="19" dataCellStyle="Percent"/>
+    <tableColumn id="14" xr3:uid="{5C9CD898-18DE-4A41-991C-EA7AFA3E2AE6}" name="rWins" dataDxfId="16" dataCellStyle="Percent"/>
     <tableColumn id="15" xr3:uid="{6F221A58-5322-4D8A-8AEB-FDBAD238A2BE}" name="Wins"/>
     <tableColumn id="16" xr3:uid="{E15C0292-EE34-4E53-B716-D74D0913B14C}" name="xWins"/>
     <tableColumn id="17" xr3:uid="{DD6780B0-11FE-4708-B152-44F8DF868344}" name="rDraws" dataDxfId="15" dataCellStyle="Percent"/>
@@ -910,23 +910,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2DA218B5-4AD2-488E-B9B2-3652EFA95102}" name="Table2" displayName="Table2" ref="A1:L26" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3" headerRowCellStyle="Check Cell">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2DA218B5-4AD2-488E-B9B2-3652EFA95102}" name="Table2" displayName="Table2" ref="A1:L26" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowCellStyle="Check Cell">
   <autoFilter ref="A1:L26" xr:uid="{2DA218B5-4AD2-488E-B9B2-3652EFA95102}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{6C8F5F25-E553-46F7-A0C3-C8FDB1C009D9}" name="Coach" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{8DE7C33B-15E4-4B44-B9F6-108F78A48B12}" name="Totals" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{6C8F5F25-E553-46F7-A0C3-C8FDB1C009D9}" name="Coach" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{8DE7C33B-15E4-4B44-B9F6-108F78A48B12}" name="Totals" dataDxfId="10">
       <calculatedColumnFormula>SUM(ABS(Table2[[#This Row],[Home Victory]]),ABS(Table2[[#This Row],[Home Draw]]),ABS(Table2[[#This Row],[Home Defeat]]),ABS(Table2[[#This Row],[Away Victory]]),ABS(Table2[[#This Row],[Away Draw]]),ABS(Table2[[#This Row],[Away Defeat]]),ABS(Table2[[#This Row],[Away Defeat]]),ABS(Table2[[#This Row],[Home Goals Conceided]]),ABS(Table2[[#This Row],[Home Goals Scored]]),ABS(Table2[[#This Row],[Away Goals Scored]]),ABS(Table2[[#This Row],[Away Goals Conceided]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5EB9EF63-EB4A-4B07-941E-BF454B6BF7AA}" name="Home Victory" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{1C0FDF4B-BEB8-4A2C-8310-9EC9FAFF1DAB}" name="Home Draw" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{FBFBAC31-F89C-45FD-B844-B04B40AAC9EA}" name="Home Defeat" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{F4339EA3-1793-4D1F-9057-66F16B1A027D}" name="Away Victory" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{37FF00CD-BD92-447E-BF39-8D78204F87A8}" name="Away Draw" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{4454C27D-BEC9-4420-BE2B-B1122B2F0852}" name="Away Defeat" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{CCE22704-3C26-4093-B98F-6EC108F4ED3A}" name="Home Goals Scored" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{90747713-CAA5-4989-8F9E-8BB7BDF94EA0}" name="Home Goals Conceided" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{65DD0F72-5906-4D7D-897C-3E315B99F9C2}" name="Away Goals Scored" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{5840234A-E15C-446C-B66F-B111C2395B8C}" name="Away Goals Conceided" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{5EB9EF63-EB4A-4B07-941E-BF454B6BF7AA}" name="Home Victory" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{1C0FDF4B-BEB8-4A2C-8310-9EC9FAFF1DAB}" name="Home Draw" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{FBFBAC31-F89C-45FD-B844-B04B40AAC9EA}" name="Home Defeat" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{F4339EA3-1793-4D1F-9057-66F16B1A027D}" name="Away Victory" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{37FF00CD-BD92-447E-BF39-8D78204F87A8}" name="Away Draw" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{4454C27D-BEC9-4420-BE2B-B1122B2F0852}" name="Away Defeat" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{CCE22704-3C26-4093-B98F-6EC108F4ED3A}" name="Home Goals Scored" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{90747713-CAA5-4989-8F9E-8BB7BDF94EA0}" name="Home Goals Conceided" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{65DD0F72-5906-4D7D-897C-3E315B99F9C2}" name="Away Goals Scored" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{5840234A-E15C-446C-B66F-B111C2395B8C}" name="Away Goals Conceided" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6492,7 +6492,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6697,7 +6697,7 @@
       <c r="G7" s="15">
         <v>0.75</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="18">
         <v>-2</v>
       </c>
       <c r="I7" s="15"/>

</xml_diff>